<commit_message>
foraminifer paper update. Diversity dependency code for foraminifera added.
</commit_message>
<xml_diff>
--- a/Evolution_Data_Mining/Cenozoic_paper/Supplementary_Data/Supplementary Table_PF_FAD_LAD_FamilyBGF.xlsx
+++ b/Evolution_Data_Mining/Cenozoic_paper/Supplementary_Data/Supplementary Table_PF_FAD_LAD_FamilyBGF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andy/Documents/projects/ML-Data Mining/Evolution_Data_Mining/Cenozoic_paper/Supplementary_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823CC7ED-9FB8-7248-9ED8-488EBAB313AA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2965DC9-3375-5147-A23E-701EF50DB1FC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20820" yWindow="460" windowWidth="20980" windowHeight="21100" xr2:uid="{91ED5034-067E-DC44-9943-A38964227778}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="32000" windowHeight="16320" xr2:uid="{91ED5034-067E-DC44-9943-A38964227778}"/>
   </bookViews>
   <sheets>
     <sheet name="PF_FAD_LAD" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,8 @@
     <sheet name="NN_turnover_prob" sheetId="7" r:id="rId7"/>
     <sheet name="NN_milancovich_oxy18events" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3283,7 +3284,7 @@
   <dimension ref="A1:F341"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A310" workbookViewId="0">
-      <selection activeCell="F179" sqref="F179"/>
+      <selection activeCell="H330" sqref="H330"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -32913,7 +32914,7 @@
         <v>0</v>
       </c>
       <c r="I709" s="28">
-        <f t="shared" ref="I709:I713" si="11">G709+H709</f>
+        <f>G709+H709</f>
         <v>0</v>
       </c>
       <c r="J709" s="18">
@@ -32946,7 +32947,7 @@
         <v>0</v>
       </c>
       <c r="I710" s="28">
-        <f t="shared" si="11"/>
+        <f>G710+H710</f>
         <v>0</v>
       </c>
       <c r="J710" s="18">
@@ -32979,7 +32980,7 @@
         <v>0</v>
       </c>
       <c r="I711" s="28">
-        <f t="shared" si="11"/>
+        <f>G711+H711</f>
         <v>0</v>
       </c>
       <c r="J711" s="18">
@@ -33012,7 +33013,7 @@
         <v>0</v>
       </c>
       <c r="I712" s="28">
-        <f t="shared" si="11"/>
+        <f>G712+H712</f>
         <v>1</v>
       </c>
       <c r="J712" s="18">
@@ -33045,7 +33046,7 @@
         <v>0</v>
       </c>
       <c r="I713" s="28">
-        <f t="shared" si="11"/>
+        <f>G713+H713</f>
         <v>0</v>
       </c>
       <c r="J713" s="18">

</xml_diff>